<commit_message>
Removed the point, and added vector. Also removed the origin and destination, it's now just a scale.
</commit_message>
<xml_diff>
--- a/EaseFormulas.xlsx
+++ b/EaseFormulas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD040A9A-A721-4463-A80E-66D86F202E5C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F855A2-91B1-419C-935D-0C20D0832CF7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>In</t>
   </si>
@@ -43,12 +43,6 @@
     <t>Cubic</t>
   </si>
   <si>
-    <t>sin((pi/2)x)</t>
-  </si>
-  <si>
-    <t>0.5+0.5sin((pi)x-(pi/2))</t>
-  </si>
-  <si>
     <t>Quadratic</t>
   </si>
   <si>
@@ -64,9 +58,6 @@
     <t>Linear</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>In Inverse</t>
   </si>
   <si>
@@ -76,109 +67,130 @@
     <t>In Out Inverse</t>
   </si>
   <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>(2asin(2y-1)+pi)/2pi</t>
-  </si>
-  <si>
-    <t>(2asin(y))/pi</t>
-  </si>
-  <si>
-    <t>1-sqrt(1-y)</t>
-  </si>
-  <si>
-    <t>sqrt(y)</t>
-  </si>
-  <si>
-    <t>y^1/3</t>
-  </si>
-  <si>
-    <t>y^1/4</t>
-  </si>
-  <si>
-    <t>y^1/5</t>
-  </si>
-  <si>
-    <t>x^2</t>
-  </si>
-  <si>
-    <t>x^3</t>
-  </si>
-  <si>
-    <t>x^4</t>
-  </si>
-  <si>
-    <t>x^5</t>
-  </si>
-  <si>
-    <t>1-sqrt(1-x^2)</t>
-  </si>
-  <si>
-    <t>0.5-0.5sqrt(1-4x^2) &amp; 0.5+0.5sqrt(1-4(x-1)^2)</t>
-  </si>
-  <si>
-    <t>1-sqrt(1-y^2)</t>
-  </si>
-  <si>
-    <t>(2asin(y-1) + pi)/pi</t>
-  </si>
-  <si>
-    <t>1+sin((pi/2)x-(pi/2))</t>
-  </si>
-  <si>
-    <t>sqrt(2y-y^2)</t>
-  </si>
-  <si>
-    <t>sqrt(y-y^2) &amp; 1-sqrt(y-y^2)</t>
-  </si>
-  <si>
-    <t>1-(1-y)^1/4</t>
-  </si>
-  <si>
-    <t>sqrt(y/2) &amp; 1-sqrt((1-y)/2)</t>
-  </si>
-  <si>
-    <t>(y/8)^1/4 &amp; 1-((1-y)/8)^1/4</t>
-  </si>
-  <si>
-    <t>sqrt(2x-x^2)</t>
-  </si>
-  <si>
-    <t>1-(x-1)^4</t>
-  </si>
-  <si>
-    <t>1-(x-1)^2</t>
-  </si>
-  <si>
-    <t>2x^2 &amp; 1-2(x-1)^2</t>
-  </si>
-  <si>
-    <t>8x^4 &amp; 1-8(x-1)^4</t>
-  </si>
-  <si>
-    <t>1-(1-x)^3</t>
-  </si>
-  <si>
-    <t>1-(1-x)^5</t>
-  </si>
-  <si>
-    <t>16x^5 &amp; 1-16(x-1)^5</t>
-  </si>
-  <si>
-    <t>4x^3 &amp; 1-4(x-1)^3</t>
-  </si>
-  <si>
-    <t>1-(1-y)^1/5</t>
-  </si>
-  <si>
-    <t>1-(1-y)^1/3</t>
-  </si>
-  <si>
-    <t>(y/4)^1/3 &amp; 1-((1-y)/4)^1/3</t>
-  </si>
-  <si>
-    <t>(y/16)^1/5 &amp; 1-((1-y)/16)^1/5</t>
+    <t>j</t>
+  </si>
+  <si>
+    <t>Scale x:</t>
+  </si>
+  <si>
+    <t>Scale y:</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>k(x/j)</t>
+  </si>
+  <si>
+    <t>k(x/j)^2</t>
+  </si>
+  <si>
+    <t>k(x/j)^3</t>
+  </si>
+  <si>
+    <t>k(x/j)^4</t>
+  </si>
+  <si>
+    <t>k(x/j)^5</t>
+  </si>
+  <si>
+    <t>k-k*sqrt(1-(x/j)^2)</t>
+  </si>
+  <si>
+    <t>k+k*sin((pi/2)(x/j)-(pi/2))</t>
+  </si>
+  <si>
+    <t>k*sin((pi/2)(x/j))</t>
+  </si>
+  <si>
+    <t>j(y/k)</t>
+  </si>
+  <si>
+    <t>j*sqrt((y/k))</t>
+  </si>
+  <si>
+    <t>j(y/k)^1/5</t>
+  </si>
+  <si>
+    <t>j(y/k)^1/4</t>
+  </si>
+  <si>
+    <t>j(y/k)^1/3</t>
+  </si>
+  <si>
+    <t>j*sqrt(2(y/k)-(y/k)^2)</t>
+  </si>
+  <si>
+    <t>k-k((x/j)-1)^2</t>
+  </si>
+  <si>
+    <t>k-k(1-(x/j))^3</t>
+  </si>
+  <si>
+    <t>k-k((x/j)-1)^4</t>
+  </si>
+  <si>
+    <t>k-k(1-(x/j))^5</t>
+  </si>
+  <si>
+    <t>k*sqrt(2(x/j)-(x/j)^2)</t>
+  </si>
+  <si>
+    <t>j(2*asin((y/k)))/pi</t>
+  </si>
+  <si>
+    <t>j-j*sqrt(1-(y/k))</t>
+  </si>
+  <si>
+    <t>j-j(1-(y/k))^1/3</t>
+  </si>
+  <si>
+    <t>j-j(1-(y/k))^1/4</t>
+  </si>
+  <si>
+    <t>j-j(1-(y/k))^1/5</t>
+  </si>
+  <si>
+    <t>j-j*sqrt(1-(y/k)^2)</t>
+  </si>
+  <si>
+    <t>(k/2)+(k/2)sin((pi)(x/j)-(pi/2))</t>
+  </si>
+  <si>
+    <t>(j/2)+j(2*asin(2(y/k)-1)+pi)/2pi</t>
+  </si>
+  <si>
+    <t>2k(x/j)^2 &amp; k-2k((x/j)-1)^2</t>
+  </si>
+  <si>
+    <t>8k(x/j)^4 &amp; k-8k((x/j)-1)^4</t>
+  </si>
+  <si>
+    <t>4k(x/j)^3 &amp; k-4k((x/j)-1)^3</t>
+  </si>
+  <si>
+    <t>16k(x/j)^5 &amp; k-16k((x/j)-1)^5</t>
+  </si>
+  <si>
+    <t>(k/2)-(k/2)sqrt(1-4(x/j)^2) &amp; (k/2)-(k/2)sqrt(1-4((x/j)-1)^2)</t>
+  </si>
+  <si>
+    <t>j*sqrt((y/k)/2) &amp; j-j*sqrt((1-(y/k))/2)</t>
+  </si>
+  <si>
+    <t>j((y/k)/4)^1/3 &amp; j-j((1-(y/k))/4)^1/3</t>
+  </si>
+  <si>
+    <t>j((y/k)/8)^1/4 &amp; j-j((1-(y/k))/8)^1/4</t>
+  </si>
+  <si>
+    <t>j((y/k)/16)^1/5 &amp; j-j((1-(y/k))/16)^1/5</t>
+  </si>
+  <si>
+    <t>j*sqrt((y/k)-(y/k)^2) &amp; j-j*sqrt((y/k)-(y/k)^2)</t>
+  </si>
+  <si>
+    <t>j + j(2*asin((y/k)-1))/pi</t>
   </si>
 </sst>
 </file>
@@ -278,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -288,6 +300,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,18 +581,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" style="6" customWidth="1"/>
-    <col min="2" max="5" width="50.7109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="63.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="86.140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="66.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
@@ -589,42 +605,42 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -632,45 +648,45 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -678,91 +694,107 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>34</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>